<commit_message>
20220513 - Atualização da planilha status
20220513
- Atualização da planilha status
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles Oliveira\OneDrive - Centro Universitário Facens\Documentos\GitHub\WebScrap\WebScrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{563419E7-110C-428D-87C8-374F3C801C95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{690E7890-CE1A-42C7-8BFE-1597F19F5BFF}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{563419E7-110C-428D-87C8-374F3C801C95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F3B558B7-B697-407F-B5A3-437336E7E611}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B2D16999-FBB7-438B-973C-B5C8C7B655F0}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Gerar colunas</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t>2-3</t>
+  </si>
+  <si>
+    <t>adicionar navegadores</t>
+  </si>
+  <si>
+    <t>adicionar clientes de email</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>Humanizar o código</t>
   </si>
 </sst>
 </file>
@@ -593,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812661A1-E6DA-48D4-8F7A-884E795647DC}">
-  <dimension ref="B2:G30"/>
+  <dimension ref="B2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AF23" sqref="AF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -722,7 +734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
@@ -730,75 +742,134 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="2" t="s">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="1" t="s">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="1" t="s">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="1" t="s">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="1" t="s">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="1" t="s">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="1" t="s">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="1" t="s">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="2"/>
+      <c r="F35" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="1">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F36" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F28" s="1">
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="1">
         <v>1</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F29" s="4" t="s">
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="F30" s="1">
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="1">
         <v>3</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -811,22 +882,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E73509E-4815-42E7-A68E-8311ADF3BD21}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1051,18 +1127,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1084,25 +1160,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE596A6-F96E-4B5E-8399-AD3154CC63EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="73df0c61-ff93-4b92-ae55-7c2c283253b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E476534-AC07-4866-9573-72163D3C3B8D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE596A6-F96E-4B5E-8399-AD3154CC63EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="73df0c61-ff93-4b92-ae55-7c2c283253b1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
20220513 - Adicionado envio de email
20220513
- Adicionado envio de email
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles Oliveira\OneDrive - Centro Universitário Facens\Documentos\GitHub\WebScrap\WebScrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{563419E7-110C-428D-87C8-374F3C801C95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F3B558B7-B697-407F-B5A3-437336E7E611}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{563419E7-110C-428D-87C8-374F3C801C95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E5A06623-199B-4F97-B19C-64EC2A98DD12}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B2D16999-FBB7-438B-973C-B5C8C7B655F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Visão geral" sheetId="1" r:id="rId1"/>
-    <sheet name="Lições aprendidas" sheetId="5" r:id="rId2"/>
-    <sheet name="Tecnologias" sheetId="6" r:id="rId3"/>
-    <sheet name="Apresentação" sheetId="2" r:id="rId4"/>
-    <sheet name="Fluxograma" sheetId="3" r:id="rId5"/>
+    <sheet name="Planilha1" sheetId="7" r:id="rId2"/>
+    <sheet name="Lições aprendidas" sheetId="5" r:id="rId3"/>
+    <sheet name="Tecnologias" sheetId="6" r:id="rId4"/>
+    <sheet name="Apresentação" sheetId="2" r:id="rId5"/>
+    <sheet name="Fluxograma" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Gerar colunas</t>
   </si>
@@ -201,6 +202,15 @@
   </si>
   <si>
     <t>Humanizar o código</t>
+  </si>
+  <si>
+    <t>Gerar relatório</t>
+  </si>
+  <si>
+    <t>Enviar e-mail com relatório anexo</t>
+  </si>
+  <si>
+    <t>Criar ambiente virtual</t>
   </si>
 </sst>
 </file>
@@ -605,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812661A1-E6DA-48D4-8F7A-884E795647DC}">
-  <dimension ref="B2:G39"/>
+  <dimension ref="B2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF23" sqref="AF23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL35" sqref="AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -734,7 +744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
@@ -742,12 +752,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
@@ -755,7 +765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
@@ -763,7 +773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
@@ -771,7 +781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
@@ -779,97 +789,112 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="2" t="s">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E26" s="1" t="s">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E27" s="1" t="s">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E28" s="1" t="s">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F29" s="1" t="s">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="F30" s="1" t="s">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E31" s="1" t="s">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="E32" s="1" t="s">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="1" t="s">
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="1" t="s">
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="2"/>
-      <c r="F35" s="1" t="s">
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" s="2"/>
+      <c r="F39" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="1">
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F40" s="1">
         <v>1</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="1">
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="F38" s="4" t="s">
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="1">
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F43" s="1">
         <v>3</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -881,6 +906,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3620233-8F27-4A0F-98E9-A44A718B2046}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E73509E-4815-42E7-A68E-8311ADF3BD21}">
   <dimension ref="B2:C4"/>
   <sheetViews>
@@ -910,7 +949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F939E82-80B4-4AE4-B181-97E4BD030032}">
   <dimension ref="B2:B8"/>
   <sheetViews>
@@ -960,7 +999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7051FD-F735-4B2D-AF0B-AE81C5624FD7}">
   <dimension ref="C2"/>
   <sheetViews>
@@ -980,7 +1019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF09093-B13F-4E84-B201-A0BF4F34E26E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1127,18 +1166,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,25 +1199,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE596A6-F96E-4B5E-8399-AD3154CC63EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="73df0c61-ff93-4b92-ae55-7c2c283253b1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E476534-AC07-4866-9573-72163D3C3B8D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE596A6-F96E-4B5E-8399-AD3154CC63EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="73df0c61-ff93-4b92-ae55-7c2c283253b1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>